<commit_message>
Fixed the BUG in NumericUpDown
</commit_message>
<xml_diff>
--- a/SSEditor/sample.xlsx
+++ b/SSEditor/sample.xlsx
@@ -7,16 +7,16 @@
     <workbookView windowWidth="19110" windowHeight="12360"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="角色成长" sheetId="1" r:id="rId1"/>
+    <sheet name="职业成长" sheetId="2" r:id="rId2"/>
+    <sheet name="计算公式" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177">
   <si>
     <t>マイユニット</t>
   </si>
@@ -280,6 +280,828 @@
   </si>
   <si>
     <t>バーサーカー</t>
+  </si>
+  <si>
+    <t>伤害</t>
+  </si>
+  <si>
+    <t>数值</t>
+  </si>
+  <si>
+    <t>公式</t>
+  </si>
+  <si>
+    <t>=(攻击力-防御力)×必杀修正</t>
+  </si>
+  <si>
+    <t>攻击力</t>
+  </si>
+  <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器攻击力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>×</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>特效修正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器级别补正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器相克修正</t>
+    </r>
+  </si>
+  <si>
+    <t>魔法</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>魔力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器攻击力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>×</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>特效修正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器级别补正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器相克修正</t>
+    </r>
+  </si>
+  <si>
+    <t>防御力</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>守备</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>地形效果</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>魔防</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>圣水效果</t>
+    </r>
+  </si>
+  <si>
+    <t>必杀修正</t>
+  </si>
+  <si>
+    <t>发动必杀时=3 通常=1</t>
+  </si>
+  <si>
+    <t>特效修正</t>
+  </si>
+  <si>
+    <t>发动特效时=3 通常=1</t>
+  </si>
+  <si>
+    <t>恢复量</t>
+  </si>
+  <si>
+    <t>有恢复效果的地形</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HP×0.2</t>
+    </r>
+  </si>
+  <si>
+    <t>ライブ</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>魔力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/2+8+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>杖级别补正</t>
+    </r>
+  </si>
+  <si>
+    <t>リブロー</t>
+  </si>
+  <si>
+    <t>リザーブ</t>
+  </si>
+  <si>
+    <t>リライブ</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>魔力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/2+15+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>杖级别补正</t>
+    </r>
+  </si>
+  <si>
+    <t>命中和必杀</t>
+  </si>
+  <si>
+    <t>实际命中率</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>命中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>回避</t>
+    </r>
+  </si>
+  <si>
+    <t>命中</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>幸运</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/2+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器命中值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器相克修正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>职业修正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>武器级别补正</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>支援效果</t>
+    </r>
+  </si>
+  <si>
+    <t>回避</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>速</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>幸运</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/2+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>地形效果</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>支援效果</t>
+    </r>
+  </si>
+  <si>
+    <t>实际必杀率</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>必杀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>必杀回避</t>
+    </r>
+  </si>
+  <si>
+    <t>必杀</t>
+  </si>
+  <si>
+    <t>技÷2＋クラス補正＋特技补正+武器的必殺値＋支援効果+职业修正</t>
+  </si>
+  <si>
+    <t>必杀回避</t>
+  </si>
+  <si>
+    <t>武器克制效果</t>
+  </si>
+  <si>
+    <t>克制侧的武器级别</t>
+  </si>
+  <si>
+    <t>立场</t>
+  </si>
+  <si>
+    <t>补正值</t>
+  </si>
+  <si>
+    <t>E D</t>
+  </si>
+  <si>
+    <t>克制</t>
+  </si>
+  <si>
+    <t>命中+5%</t>
+  </si>
+  <si>
+    <t>被克</t>
+  </si>
+  <si>
+    <t>命中-5%</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>命中+10%</t>
+  </si>
+  <si>
+    <t>命中-10%</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>攻击+1</t>
+  </si>
+  <si>
+    <t>攻击-1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>命中+15%</t>
+  </si>
+  <si>
+    <t>命中-15%</t>
+  </si>
+  <si>
+    <t>地形效果</t>
+  </si>
+  <si>
+    <t>地形</t>
+  </si>
+  <si>
+    <t>恢复</t>
+  </si>
+  <si>
+    <t>林</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>山</t>
+  </si>
+  <si>
+    <t>高山</t>
+  </si>
+  <si>
+    <t>村</t>
+  </si>
+  <si>
+    <t>废墟</t>
+  </si>
+  <si>
+    <t>海</t>
+  </si>
+  <si>
+    <t>柱</t>
+  </si>
+  <si>
+    <t>砦</t>
+  </si>
+  <si>
+    <t>城门</t>
+  </si>
+  <si>
+    <t>玉座</t>
+  </si>
+  <si>
+    <t>武器级别补正</t>
+  </si>
+  <si>
+    <t>武器</t>
+  </si>
+  <si>
+    <t>剑</t>
+  </si>
+  <si>
+    <t>攻击+2</t>
+  </si>
+  <si>
+    <t>攻击+3</t>
+  </si>
+  <si>
+    <t>枪</t>
+  </si>
+  <si>
+    <t>命中+5%，攻击+1</t>
+  </si>
+  <si>
+    <t>命中+5%，攻击+2</t>
+  </si>
+  <si>
+    <t>斧</t>
+  </si>
+  <si>
+    <t>攻击+1，命中+10%</t>
+  </si>
+  <si>
+    <t>弓</t>
+  </si>
+  <si>
+    <t>杖</t>
+  </si>
+  <si>
+    <t>恢复量+1</t>
+  </si>
+  <si>
+    <t>恢复量+2</t>
+  </si>
+  <si>
+    <t>恢复量+3</t>
+  </si>
+  <si>
+    <t>攻速判定</t>
+  </si>
+  <si>
+    <t>攻击速度</t>
+  </si>
+  <si>
+    <r>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>速</t>
+    </r>
+  </si>
+  <si>
+    <t>追击发动条件</t>
+  </si>
+  <si>
+    <t>=(自己的攻击速度)-(对手的攻击速度)≥5</t>
   </si>
 </sst>
 </file>
@@ -287,15 +1109,33 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="4"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="0"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -303,14 +1143,18 @@
       <sz val="9"/>
       <color indexed="1"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -327,12 +1171,186 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="0"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -371,18 +1389,81 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -697,11 +1778,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -728,7 +1809,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -737,31 +1818,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3">
-        <v>40</v>
-      </c>
-      <c r="D1" s="3">
-        <v>35</v>
-      </c>
-      <c r="E1" s="3">
-        <v>35</v>
-      </c>
-      <c r="F1" s="3">
-        <v>35</v>
-      </c>
-      <c r="G1" s="3">
+      <c r="B1" s="22">
+        <v>40</v>
+      </c>
+      <c r="C1" s="22">
+        <v>40</v>
+      </c>
+      <c r="D1" s="22">
+        <v>35</v>
+      </c>
+      <c r="E1" s="22">
+        <v>35</v>
+      </c>
+      <c r="F1" s="22">
+        <v>35</v>
+      </c>
+      <c r="G1" s="22">
         <v>55</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="22">
         <v>30</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="22">
         <v>20</v>
       </c>
       <c r="J1">
@@ -770,31 +1851,31 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>45</v>
-      </c>
-      <c r="C2" s="3">
-        <v>40</v>
-      </c>
-      <c r="D2" s="3">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3">
-        <v>40</v>
-      </c>
-      <c r="F2" s="3">
-        <v>40</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="B2" s="22">
+        <v>45</v>
+      </c>
+      <c r="C2" s="22">
+        <v>40</v>
+      </c>
+      <c r="D2" s="22">
+        <v>10</v>
+      </c>
+      <c r="E2" s="22">
+        <v>40</v>
+      </c>
+      <c r="F2" s="22">
+        <v>40</v>
+      </c>
+      <c r="G2" s="22">
         <v>70</v>
       </c>
-      <c r="H2" s="3">
-        <v>35</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="H2" s="22">
+        <v>35</v>
+      </c>
+      <c r="I2" s="22">
         <v>20</v>
       </c>
       <c r="J2">
@@ -803,31 +1884,31 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="22">
         <v>60</v>
       </c>
-      <c r="C3" s="3">
-        <v>40</v>
-      </c>
-      <c r="D3" s="3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
-        <v>40</v>
-      </c>
-      <c r="F3" s="3">
-        <v>35</v>
-      </c>
-      <c r="G3" s="3">
-        <v>40</v>
-      </c>
-      <c r="H3" s="3">
-        <v>40</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="C3" s="22">
+        <v>40</v>
+      </c>
+      <c r="D3" s="22">
+        <v>10</v>
+      </c>
+      <c r="E3" s="22">
+        <v>40</v>
+      </c>
+      <c r="F3" s="22">
+        <v>35</v>
+      </c>
+      <c r="G3" s="22">
+        <v>40</v>
+      </c>
+      <c r="H3" s="22">
+        <v>40</v>
+      </c>
+      <c r="I3" s="22">
         <v>20</v>
       </c>
       <c r="J3">
@@ -836,31 +1917,31 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>35</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="22">
+        <v>35</v>
+      </c>
+      <c r="C4" s="22">
         <v>25</v>
       </c>
-      <c r="D4" s="3">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="22">
+        <v>35</v>
+      </c>
+      <c r="E4" s="22">
         <v>30</v>
       </c>
-      <c r="F4" s="3">
-        <v>35</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="22">
+        <v>35</v>
+      </c>
+      <c r="G4" s="22">
         <v>65</v>
       </c>
-      <c r="H4" s="3">
-        <v>15</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="H4" s="22">
+        <v>15</v>
+      </c>
+      <c r="I4" s="22">
         <v>35</v>
       </c>
       <c r="J4">
@@ -869,31 +1950,31 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3">
-        <v>40</v>
-      </c>
-      <c r="F5" s="3">
-        <v>40</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="B5" s="22">
+        <v>40</v>
+      </c>
+      <c r="C5" s="22">
+        <v>35</v>
+      </c>
+      <c r="D5" s="22">
+        <v>20</v>
+      </c>
+      <c r="E5" s="22">
+        <v>40</v>
+      </c>
+      <c r="F5" s="22">
+        <v>40</v>
+      </c>
+      <c r="G5" s="22">
         <v>60</v>
       </c>
-      <c r="H5" s="3">
-        <v>35</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="H5" s="22">
+        <v>35</v>
+      </c>
+      <c r="I5" s="22">
         <v>20</v>
       </c>
       <c r="J5">
@@ -902,31 +1983,31 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3">
-        <v>40</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="B6" s="22">
+        <v>35</v>
+      </c>
+      <c r="C6" s="22">
+        <v>40</v>
+      </c>
+      <c r="D6" s="22">
         <v>30</v>
       </c>
-      <c r="E6" s="3">
-        <v>40</v>
-      </c>
-      <c r="F6" s="3">
-        <v>45</v>
-      </c>
-      <c r="G6" s="3">
-        <v>40</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="E6" s="22">
+        <v>40</v>
+      </c>
+      <c r="F6" s="22">
+        <v>45</v>
+      </c>
+      <c r="G6" s="22">
+        <v>40</v>
+      </c>
+      <c r="H6" s="22">
         <v>25</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="22">
         <v>25</v>
       </c>
       <c r="J6">
@@ -935,31 +2016,31 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="22">
         <v>50</v>
       </c>
-      <c r="C7" s="3">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3">
-        <v>35</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="C7" s="22">
+        <v>45</v>
+      </c>
+      <c r="D7" s="22">
+        <v>10</v>
+      </c>
+      <c r="E7" s="22">
+        <v>35</v>
+      </c>
+      <c r="F7" s="22">
         <v>30</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="22">
         <v>50</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="22">
         <v>50</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="22">
         <v>10</v>
       </c>
       <c r="J7">
@@ -968,31 +2049,31 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="22">
         <v>60</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="22">
         <v>50</v>
       </c>
-      <c r="D8" s="3">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3">
-        <v>45</v>
-      </c>
-      <c r="F8" s="3">
-        <v>35</v>
-      </c>
-      <c r="G8" s="3">
-        <v>45</v>
-      </c>
-      <c r="H8" s="3">
-        <v>40</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="D8" s="22">
+        <v>10</v>
+      </c>
+      <c r="E8" s="22">
+        <v>45</v>
+      </c>
+      <c r="F8" s="22">
+        <v>35</v>
+      </c>
+      <c r="G8" s="22">
+        <v>45</v>
+      </c>
+      <c r="H8" s="22">
+        <v>40</v>
+      </c>
+      <c r="I8" s="22">
         <v>5</v>
       </c>
       <c r="J8">
@@ -1001,31 +2082,31 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3">
-        <v>40</v>
-      </c>
-      <c r="E9" s="3">
-        <v>40</v>
-      </c>
-      <c r="F9" s="3">
-        <v>40</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="B9" s="22">
+        <v>35</v>
+      </c>
+      <c r="C9" s="22">
+        <v>15</v>
+      </c>
+      <c r="D9" s="22">
+        <v>40</v>
+      </c>
+      <c r="E9" s="22">
+        <v>40</v>
+      </c>
+      <c r="F9" s="22">
+        <v>40</v>
+      </c>
+      <c r="G9" s="22">
         <v>50</v>
       </c>
-      <c r="H9" s="3">
-        <v>20</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="H9" s="22">
+        <v>20</v>
+      </c>
+      <c r="I9" s="22">
         <v>30</v>
       </c>
       <c r="J9">
@@ -1034,31 +2115,31 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="22">
         <v>50</v>
       </c>
-      <c r="C10" s="3">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3">
-        <v>40</v>
-      </c>
-      <c r="F10" s="3">
-        <v>35</v>
-      </c>
-      <c r="G10" s="3">
-        <v>35</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="C10" s="22">
+        <v>40</v>
+      </c>
+      <c r="D10" s="22">
+        <v>15</v>
+      </c>
+      <c r="E10" s="22">
+        <v>40</v>
+      </c>
+      <c r="F10" s="22">
+        <v>35</v>
+      </c>
+      <c r="G10" s="22">
+        <v>35</v>
+      </c>
+      <c r="H10" s="22">
         <v>55</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="22">
         <v>30</v>
       </c>
       <c r="J10">
@@ -1067,31 +2148,31 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="A11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22">
+        <v>35</v>
+      </c>
+      <c r="C11" s="22">
         <v>30</v>
       </c>
-      <c r="D11" s="3">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3">
-        <v>45</v>
-      </c>
-      <c r="F11" s="3">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="D11" s="22">
+        <v>20</v>
+      </c>
+      <c r="E11" s="22">
+        <v>45</v>
+      </c>
+      <c r="F11" s="22">
+        <v>45</v>
+      </c>
+      <c r="G11" s="22">
         <v>60</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="22">
         <v>25</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="22">
         <v>30</v>
       </c>
       <c r="J11">
@@ -1100,31 +2181,31 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="B12" s="22">
+        <v>40</v>
+      </c>
+      <c r="C12" s="22">
+        <v>35</v>
+      </c>
+      <c r="D12" s="22">
+        <v>20</v>
+      </c>
+      <c r="E12" s="22">
         <v>50</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="22">
         <v>50</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="22">
         <v>55</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="22">
         <v>25</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="22">
         <v>20</v>
       </c>
       <c r="J12">
@@ -1133,31 +2214,31 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="22">
         <v>50</v>
       </c>
-      <c r="C13" s="3">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3">
-        <v>35</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="C13" s="22">
+        <v>20</v>
+      </c>
+      <c r="D13" s="22">
+        <v>35</v>
+      </c>
+      <c r="E13" s="22">
         <v>30</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="22">
         <v>30</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="22">
         <v>65</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="22">
         <v>30</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="22">
         <v>25</v>
       </c>
       <c r="J13">
@@ -1166,31 +2247,31 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="22">
         <v>30</v>
       </c>
-      <c r="C14" s="3">
-        <v>20</v>
-      </c>
-      <c r="D14" s="3">
-        <v>40</v>
-      </c>
-      <c r="E14" s="3">
-        <v>40</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="C14" s="22">
+        <v>20</v>
+      </c>
+      <c r="D14" s="22">
+        <v>40</v>
+      </c>
+      <c r="E14" s="22">
+        <v>40</v>
+      </c>
+      <c r="F14" s="22">
         <v>30</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="22">
         <v>80</v>
       </c>
-      <c r="H14" s="3">
-        <v>10</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="H14" s="22">
+        <v>10</v>
+      </c>
+      <c r="I14" s="22">
         <v>40</v>
       </c>
       <c r="J14">
@@ -1199,31 +2280,31 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="22">
         <v>50</v>
       </c>
-      <c r="C15" s="3">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3">
-        <v>15</v>
-      </c>
-      <c r="E15" s="3">
-        <v>45</v>
-      </c>
-      <c r="F15" s="3">
-        <v>45</v>
-      </c>
-      <c r="G15" s="3">
-        <v>35</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="C15" s="22">
+        <v>45</v>
+      </c>
+      <c r="D15" s="22">
+        <v>15</v>
+      </c>
+      <c r="E15" s="22">
+        <v>45</v>
+      </c>
+      <c r="F15" s="22">
+        <v>45</v>
+      </c>
+      <c r="G15" s="22">
+        <v>35</v>
+      </c>
+      <c r="H15" s="22">
         <v>25</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="22">
         <v>15</v>
       </c>
       <c r="J15">
@@ -1232,31 +2313,31 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22">
         <v>60</v>
       </c>
-      <c r="C16" s="3">
-        <v>45</v>
-      </c>
-      <c r="D16" s="3">
-        <v>15</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="C16" s="22">
+        <v>45</v>
+      </c>
+      <c r="D16" s="22">
+        <v>15</v>
+      </c>
+      <c r="E16" s="22">
         <v>50</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="22">
         <v>55</v>
       </c>
-      <c r="G16" s="3">
-        <v>40</v>
-      </c>
-      <c r="H16" s="3">
-        <v>40</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="G16" s="22">
+        <v>40</v>
+      </c>
+      <c r="H16" s="22">
+        <v>40</v>
+      </c>
+      <c r="I16" s="22">
         <v>15</v>
       </c>
       <c r="J16">
@@ -1265,31 +2346,31 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="22">
         <v>50</v>
       </c>
-      <c r="C17" s="3">
-        <v>45</v>
-      </c>
-      <c r="D17" s="3">
-        <v>15</v>
-      </c>
-      <c r="E17" s="3">
-        <v>35</v>
-      </c>
-      <c r="F17" s="3">
-        <v>35</v>
-      </c>
-      <c r="G17" s="3">
-        <v>45</v>
-      </c>
-      <c r="H17" s="3">
-        <v>40</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="C17" s="22">
+        <v>45</v>
+      </c>
+      <c r="D17" s="22">
+        <v>15</v>
+      </c>
+      <c r="E17" s="22">
+        <v>35</v>
+      </c>
+      <c r="F17" s="22">
+        <v>35</v>
+      </c>
+      <c r="G17" s="22">
+        <v>45</v>
+      </c>
+      <c r="H17" s="22">
+        <v>40</v>
+      </c>
+      <c r="I17" s="22">
         <v>25</v>
       </c>
       <c r="J17">
@@ -1298,31 +2379,31 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="22">
         <v>70</v>
       </c>
-      <c r="C18" s="3">
-        <v>45</v>
-      </c>
-      <c r="D18" s="3">
-        <v>35</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="C18" s="22">
+        <v>45</v>
+      </c>
+      <c r="D18" s="22">
+        <v>35</v>
+      </c>
+      <c r="E18" s="22">
         <v>30</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="22">
         <v>30</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="22">
         <v>65</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="22">
         <v>50</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="22">
         <v>35</v>
       </c>
       <c r="J18">
@@ -1331,31 +2412,31 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="22">
         <v>60</v>
       </c>
-      <c r="C19" s="3">
-        <v>40</v>
-      </c>
-      <c r="D19" s="3">
-        <v>10</v>
-      </c>
-      <c r="E19" s="3">
-        <v>40</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="C19" s="22">
+        <v>40</v>
+      </c>
+      <c r="D19" s="22">
+        <v>10</v>
+      </c>
+      <c r="E19" s="22">
+        <v>40</v>
+      </c>
+      <c r="F19" s="22">
         <v>30</v>
       </c>
-      <c r="G19" s="3">
-        <v>45</v>
-      </c>
-      <c r="H19" s="3">
-        <v>40</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="G19" s="22">
+        <v>45</v>
+      </c>
+      <c r="H19" s="22">
+        <v>40</v>
+      </c>
+      <c r="I19" s="22">
         <v>10</v>
       </c>
       <c r="J19">
@@ -1364,31 +2445,31 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="22">
+        <v>40</v>
+      </c>
+      <c r="C20" s="22">
         <v>25</v>
       </c>
-      <c r="D20" s="3">
-        <v>45</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D20" s="22">
+        <v>45</v>
+      </c>
+      <c r="E20" s="22">
         <v>25</v>
       </c>
-      <c r="F20" s="3">
-        <v>45</v>
-      </c>
-      <c r="G20" s="3">
-        <v>40</v>
-      </c>
-      <c r="H20" s="3">
-        <v>35</v>
-      </c>
-      <c r="I20" s="3">
+      <c r="F20" s="22">
+        <v>45</v>
+      </c>
+      <c r="G20" s="22">
+        <v>40</v>
+      </c>
+      <c r="H20" s="22">
+        <v>35</v>
+      </c>
+      <c r="I20" s="22">
         <v>20</v>
       </c>
       <c r="J20">
@@ -1397,31 +2478,31 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="A21" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22">
+        <v>45</v>
+      </c>
+      <c r="C21" s="22">
         <v>25</v>
       </c>
-      <c r="D21" s="3">
-        <v>35</v>
-      </c>
-      <c r="E21" s="3">
-        <v>45</v>
-      </c>
-      <c r="F21" s="3">
-        <v>35</v>
-      </c>
-      <c r="G21" s="3">
-        <v>45</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="D21" s="22">
+        <v>35</v>
+      </c>
+      <c r="E21" s="22">
+        <v>45</v>
+      </c>
+      <c r="F21" s="22">
+        <v>35</v>
+      </c>
+      <c r="G21" s="22">
+        <v>45</v>
+      </c>
+      <c r="H21" s="22">
         <v>25</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="22">
         <v>30</v>
       </c>
       <c r="J21">
@@ -1430,31 +2511,31 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3">
-        <v>35</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="B22" s="22">
+        <v>40</v>
+      </c>
+      <c r="C22" s="22">
+        <v>35</v>
+      </c>
+      <c r="D22" s="22">
         <v>25</v>
       </c>
-      <c r="E22" s="3">
-        <v>45</v>
-      </c>
-      <c r="F22" s="3">
-        <v>45</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="E22" s="22">
+        <v>45</v>
+      </c>
+      <c r="F22" s="22">
+        <v>45</v>
+      </c>
+      <c r="G22" s="22">
         <v>60</v>
       </c>
-      <c r="H22" s="3">
-        <v>20</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="H22" s="22">
+        <v>20</v>
+      </c>
+      <c r="I22" s="22">
         <v>20</v>
       </c>
       <c r="J22">
@@ -1463,31 +2544,31 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="22">
         <v>55</v>
       </c>
-      <c r="C23" s="3">
-        <v>40</v>
-      </c>
-      <c r="D23" s="3">
-        <v>20</v>
-      </c>
-      <c r="E23" s="3">
-        <v>40</v>
-      </c>
-      <c r="F23" s="3">
-        <v>35</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="C23" s="22">
+        <v>40</v>
+      </c>
+      <c r="D23" s="22">
+        <v>20</v>
+      </c>
+      <c r="E23" s="22">
+        <v>40</v>
+      </c>
+      <c r="F23" s="22">
+        <v>35</v>
+      </c>
+      <c r="G23" s="22">
         <v>50</v>
       </c>
-      <c r="H23" s="3">
-        <v>45</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="H23" s="22">
+        <v>45</v>
+      </c>
+      <c r="I23" s="22">
         <v>10</v>
       </c>
       <c r="J23">
@@ -1496,31 +2577,31 @@
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>45</v>
-      </c>
-      <c r="C24" s="3">
-        <v>35</v>
-      </c>
-      <c r="D24" s="3">
-        <v>35</v>
-      </c>
-      <c r="E24" s="3">
-        <v>45</v>
-      </c>
-      <c r="F24" s="3">
-        <v>40</v>
-      </c>
-      <c r="G24" s="3">
-        <v>40</v>
-      </c>
-      <c r="H24" s="3">
-        <v>40</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="B24" s="22">
+        <v>45</v>
+      </c>
+      <c r="C24" s="22">
+        <v>35</v>
+      </c>
+      <c r="D24" s="22">
+        <v>35</v>
+      </c>
+      <c r="E24" s="22">
+        <v>45</v>
+      </c>
+      <c r="F24" s="22">
+        <v>40</v>
+      </c>
+      <c r="G24" s="22">
+        <v>40</v>
+      </c>
+      <c r="H24" s="22">
+        <v>40</v>
+      </c>
+      <c r="I24" s="22">
         <v>20</v>
       </c>
       <c r="J24">
@@ -1529,31 +2610,31 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="22">
         <v>50</v>
       </c>
-      <c r="C25" s="3">
-        <v>35</v>
-      </c>
-      <c r="D25" s="3">
-        <v>20</v>
-      </c>
-      <c r="E25" s="3">
-        <v>40</v>
-      </c>
-      <c r="F25" s="3">
-        <v>40</v>
-      </c>
-      <c r="G25" s="3">
-        <v>45</v>
-      </c>
-      <c r="H25" s="3">
-        <v>35</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="C25" s="22">
+        <v>35</v>
+      </c>
+      <c r="D25" s="22">
+        <v>20</v>
+      </c>
+      <c r="E25" s="22">
+        <v>40</v>
+      </c>
+      <c r="F25" s="22">
+        <v>40</v>
+      </c>
+      <c r="G25" s="22">
+        <v>45</v>
+      </c>
+      <c r="H25" s="22">
+        <v>35</v>
+      </c>
+      <c r="I25" s="22">
         <v>30</v>
       </c>
       <c r="J25">
@@ -1562,31 +2643,31 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="22">
         <v>65</v>
       </c>
-      <c r="C26" s="3">
-        <v>45</v>
-      </c>
-      <c r="D26" s="3">
-        <v>10</v>
-      </c>
-      <c r="E26" s="3">
-        <v>40</v>
-      </c>
-      <c r="F26" s="3">
-        <v>35</v>
-      </c>
-      <c r="G26" s="3">
-        <v>45</v>
-      </c>
-      <c r="H26" s="3">
-        <v>40</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="C26" s="22">
+        <v>45</v>
+      </c>
+      <c r="D26" s="22">
+        <v>10</v>
+      </c>
+      <c r="E26" s="22">
+        <v>40</v>
+      </c>
+      <c r="F26" s="22">
+        <v>35</v>
+      </c>
+      <c r="G26" s="22">
+        <v>45</v>
+      </c>
+      <c r="H26" s="22">
+        <v>40</v>
+      </c>
+      <c r="I26" s="22">
         <v>15</v>
       </c>
       <c r="J26">
@@ -1595,31 +2676,31 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="22">
         <v>50</v>
       </c>
-      <c r="C27" s="3">
-        <v>35</v>
-      </c>
-      <c r="D27" s="3">
-        <v>20</v>
-      </c>
-      <c r="E27" s="3">
-        <v>45</v>
-      </c>
-      <c r="F27" s="3">
-        <v>45</v>
-      </c>
-      <c r="G27" s="3">
+      <c r="C27" s="22">
+        <v>35</v>
+      </c>
+      <c r="D27" s="22">
+        <v>20</v>
+      </c>
+      <c r="E27" s="22">
+        <v>45</v>
+      </c>
+      <c r="F27" s="22">
+        <v>45</v>
+      </c>
+      <c r="G27" s="22">
         <v>55</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="22">
         <v>30</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="22">
         <v>25</v>
       </c>
       <c r="J27">
@@ -1628,31 +2709,31 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="22">
         <v>50</v>
       </c>
-      <c r="C28" s="3">
-        <v>45</v>
-      </c>
-      <c r="D28" s="3">
-        <v>15</v>
-      </c>
-      <c r="E28" s="3">
-        <v>40</v>
-      </c>
-      <c r="F28" s="3">
-        <v>45</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="C28" s="22">
+        <v>45</v>
+      </c>
+      <c r="D28" s="22">
+        <v>15</v>
+      </c>
+      <c r="E28" s="22">
+        <v>40</v>
+      </c>
+      <c r="F28" s="22">
+        <v>45</v>
+      </c>
+      <c r="G28" s="22">
         <v>80</v>
       </c>
-      <c r="H28" s="3">
-        <v>35</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="H28" s="22">
+        <v>35</v>
+      </c>
+      <c r="I28" s="22">
         <v>15</v>
       </c>
       <c r="J28">
@@ -1661,31 +2742,31 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>45</v>
-      </c>
-      <c r="C29" s="3">
+      <c r="B29" s="22">
+        <v>45</v>
+      </c>
+      <c r="C29" s="22">
         <v>30</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="22">
         <v>30</v>
       </c>
-      <c r="E29" s="3">
-        <v>35</v>
-      </c>
-      <c r="F29" s="3">
-        <v>35</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="E29" s="22">
+        <v>35</v>
+      </c>
+      <c r="F29" s="22">
+        <v>35</v>
+      </c>
+      <c r="G29" s="22">
         <v>80</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="22">
         <v>30</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="22">
         <v>30</v>
       </c>
       <c r="J29">
@@ -1694,31 +2775,31 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="22">
         <v>80</v>
       </c>
-      <c r="C30" s="3">
-        <v>40</v>
-      </c>
-      <c r="D30" s="3">
-        <v>40</v>
-      </c>
-      <c r="E30" s="3">
-        <v>35</v>
-      </c>
-      <c r="F30" s="3">
+      <c r="C30" s="22">
+        <v>40</v>
+      </c>
+      <c r="D30" s="22">
+        <v>40</v>
+      </c>
+      <c r="E30" s="22">
+        <v>35</v>
+      </c>
+      <c r="F30" s="22">
         <v>30</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="22">
         <v>80</v>
       </c>
-      <c r="H30" s="3">
-        <v>45</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="H30" s="22">
+        <v>45</v>
+      </c>
+      <c r="I30" s="22">
         <v>45</v>
       </c>
       <c r="J30">
@@ -1727,31 +2808,31 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>45</v>
-      </c>
-      <c r="C31" s="3">
-        <v>45</v>
-      </c>
-      <c r="D31" s="3">
-        <v>35</v>
-      </c>
-      <c r="E31" s="3">
-        <v>45</v>
-      </c>
-      <c r="F31" s="3">
-        <v>45</v>
-      </c>
-      <c r="G31" s="3">
-        <v>35</v>
-      </c>
-      <c r="H31" s="3">
-        <v>35</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="B31" s="22">
+        <v>45</v>
+      </c>
+      <c r="C31" s="22">
+        <v>45</v>
+      </c>
+      <c r="D31" s="22">
+        <v>35</v>
+      </c>
+      <c r="E31" s="22">
+        <v>45</v>
+      </c>
+      <c r="F31" s="22">
+        <v>45</v>
+      </c>
+      <c r="G31" s="22">
+        <v>35</v>
+      </c>
+      <c r="H31" s="22">
+        <v>35</v>
+      </c>
+      <c r="I31" s="22">
         <v>35</v>
       </c>
       <c r="J31">
@@ -1760,31 +2841,31 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="22">
         <v>70</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="22">
         <v>60</v>
       </c>
-      <c r="D32" s="3">
-        <v>10</v>
-      </c>
-      <c r="E32" s="3">
-        <v>35</v>
-      </c>
-      <c r="F32" s="3">
-        <v>35</v>
-      </c>
-      <c r="G32" s="3">
-        <v>45</v>
-      </c>
-      <c r="H32" s="3">
-        <v>45</v>
-      </c>
-      <c r="I32" s="3">
+      <c r="D32" s="22">
+        <v>10</v>
+      </c>
+      <c r="E32" s="22">
+        <v>35</v>
+      </c>
+      <c r="F32" s="22">
+        <v>35</v>
+      </c>
+      <c r="G32" s="22">
+        <v>45</v>
+      </c>
+      <c r="H32" s="22">
+        <v>45</v>
+      </c>
+      <c r="I32" s="22">
         <v>30</v>
       </c>
       <c r="J32">
@@ -1793,31 +2874,31 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>40</v>
-      </c>
-      <c r="C33" s="3">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3">
+      <c r="B33" s="22">
+        <v>40</v>
+      </c>
+      <c r="C33" s="22">
+        <v>10</v>
+      </c>
+      <c r="D33" s="22">
         <v>60</v>
       </c>
-      <c r="E33" s="3">
-        <v>45</v>
-      </c>
-      <c r="F33" s="3">
-        <v>45</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="E33" s="22">
+        <v>45</v>
+      </c>
+      <c r="F33" s="22">
+        <v>45</v>
+      </c>
+      <c r="G33" s="22">
         <v>70</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="22">
         <v>30</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="22">
         <v>35</v>
       </c>
       <c r="J33">
@@ -1826,31 +2907,31 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="22">
         <v>60</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="22">
         <v>50</v>
       </c>
-      <c r="D34" s="3">
-        <v>10</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="22">
+        <v>10</v>
+      </c>
+      <c r="E34" s="22">
         <v>50</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="22">
         <v>50</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="22">
         <v>60</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="22">
         <v>30</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="22">
         <v>10</v>
       </c>
       <c r="J34">
@@ -1859,31 +2940,31 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
-        <v>45</v>
-      </c>
-      <c r="C35" s="3">
+      <c r="B35" s="22">
+        <v>45</v>
+      </c>
+      <c r="C35" s="22">
         <v>30</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="22">
         <v>50</v>
       </c>
-      <c r="E35" s="3">
-        <v>35</v>
-      </c>
-      <c r="F35" s="3">
-        <v>45</v>
-      </c>
-      <c r="G35" s="3">
+      <c r="E35" s="22">
+        <v>35</v>
+      </c>
+      <c r="F35" s="22">
+        <v>45</v>
+      </c>
+      <c r="G35" s="22">
         <v>60</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="22">
         <v>30</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="22">
         <v>35</v>
       </c>
       <c r="J35">
@@ -1892,7 +2973,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -1913,33 +2994,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B2">
@@ -1999,7 +3080,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B4">
@@ -2059,7 +3140,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B6">
@@ -2119,7 +3200,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B8">
@@ -2179,7 +3260,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B10">
@@ -2239,7 +3320,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="21" t="s">
         <v>53</v>
       </c>
       <c r="B12">
@@ -2299,7 +3380,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B14">
@@ -2359,7 +3440,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B16">
@@ -2419,7 +3500,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B18">
@@ -2479,7 +3560,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B20">
@@ -2539,7 +3620,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B22">
@@ -2599,28 +3680,28 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F24" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2655,7 +3736,7 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B26">
@@ -2715,7 +3796,7 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B28">
@@ -2775,7 +3856,7 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B30">
@@ -2835,7 +3916,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B32">
@@ -2895,7 +3976,7 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B34">
@@ -2955,7 +4036,7 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="21" t="s">
         <v>76</v>
       </c>
       <c r="B36">
@@ -3015,7 +4096,7 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="21" t="s">
         <v>78</v>
       </c>
       <c r="B38">
@@ -3075,7 +4156,7 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B40">
@@ -3135,7 +4216,7 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B42">
@@ -3195,7 +4276,7 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B44">
@@ -3255,7 +4336,7 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B46">
@@ -3315,466 +4396,466 @@
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="2"/>
+      <c r="A48" s="21"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="2"/>
+      <c r="A50" s="21"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="2"/>
+      <c r="A52" s="21"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="2"/>
+      <c r="A54" s="21"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="2"/>
+      <c r="A56" s="21"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="2"/>
+      <c r="A58" s="21"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="2"/>
+      <c r="A60" s="21"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="2"/>
+      <c r="A62" s="21"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="2"/>
+      <c r="A64" s="21"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="2"/>
+      <c r="A66" s="21"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="2"/>
+      <c r="A68" s="21"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="2"/>
+      <c r="A70" s="21"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="2"/>
+      <c r="A72" s="21"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="2"/>
+      <c r="A74" s="21"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="2"/>
+      <c r="A76" s="21"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="2"/>
+      <c r="A78" s="21"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="2"/>
+      <c r="A80" s="21"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="2"/>
+      <c r="A82" s="21"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="2"/>
+      <c r="A84" s="21"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="2"/>
+      <c r="A86" s="21"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="2"/>
+      <c r="A88" s="21"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="2"/>
+      <c r="A90" s="21"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="2"/>
+      <c r="A92" s="21"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="2"/>
+      <c r="A94" s="21"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="2"/>
+      <c r="A96" s="21"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="2"/>
+      <c r="A98" s="21"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="2"/>
+      <c r="A100" s="21"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="2"/>
+      <c r="A102" s="21"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="2"/>
+      <c r="A104" s="21"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="2"/>
+      <c r="A106" s="21"/>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="2"/>
+      <c r="A108" s="21"/>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="2"/>
+      <c r="A110" s="21"/>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="2"/>
+      <c r="A112" s="21"/>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="2"/>
+      <c r="A114" s="21"/>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="2"/>
+      <c r="A116" s="21"/>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="2"/>
+      <c r="A118" s="21"/>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="2"/>
+      <c r="A120" s="21"/>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="2"/>
+      <c r="A122" s="21"/>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="2"/>
+      <c r="A124" s="21"/>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="2"/>
+      <c r="A126" s="21"/>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="2"/>
+      <c r="A128" s="21"/>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="2"/>
+      <c r="A130" s="21"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="2"/>
+      <c r="A132" s="21"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="2"/>
+      <c r="A134" s="21"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="2"/>
+      <c r="A136" s="21"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="2"/>
+      <c r="A138" s="21"/>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="2"/>
+      <c r="A140" s="21"/>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="2"/>
+      <c r="A142" s="21"/>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="2"/>
+      <c r="A144" s="21"/>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="2"/>
+      <c r="A146" s="21"/>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="2"/>
+      <c r="A148" s="21"/>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="2"/>
+      <c r="A150" s="21"/>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="2"/>
+      <c r="A152" s="21"/>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="2"/>
+      <c r="A154" s="21"/>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="2"/>
+      <c r="A156" s="21"/>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="2"/>
+      <c r="A158" s="21"/>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="2"/>
+      <c r="A160" s="21"/>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="2"/>
+      <c r="A162" s="21"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="2"/>
+      <c r="A164" s="21"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="2"/>
+      <c r="A166" s="21"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="2"/>
+      <c r="A168" s="21"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="2"/>
+      <c r="A170" s="21"/>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="2"/>
+      <c r="A172" s="21"/>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="2"/>
+      <c r="A174" s="21"/>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="2"/>
+      <c r="A176" s="21"/>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="2"/>
+      <c r="A178" s="21"/>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="2"/>
+      <c r="A180" s="21"/>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="2"/>
+      <c r="A182" s="21"/>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="2"/>
+      <c r="A184" s="21"/>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="2"/>
+      <c r="A186" s="21"/>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="2"/>
+      <c r="A188" s="21"/>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="2"/>
+      <c r="A190" s="21"/>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="2"/>
+      <c r="A192" s="21"/>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="2"/>
+      <c r="A194" s="21"/>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="2"/>
+      <c r="A196" s="21"/>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="2"/>
+      <c r="A198" s="21"/>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="2"/>
+      <c r="A200" s="21"/>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="2"/>
+      <c r="A202" s="21"/>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="2"/>
+      <c r="A204" s="21"/>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="2"/>
+      <c r="A206" s="21"/>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="2"/>
+      <c r="A208" s="21"/>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="2"/>
+      <c r="A210" s="21"/>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="2"/>
+      <c r="A212" s="21"/>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="2"/>
+      <c r="A214" s="21"/>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="2"/>
+      <c r="A216" s="21"/>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="2"/>
+      <c r="A218" s="21"/>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="2"/>
+      <c r="A220" s="21"/>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="2"/>
+      <c r="A222" s="21"/>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="2"/>
+      <c r="A224" s="21"/>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="2"/>
+      <c r="A226" s="21"/>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="2"/>
+      <c r="A228" s="21"/>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="2"/>
+      <c r="A230" s="21"/>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="2"/>
+      <c r="A232" s="21"/>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="2"/>
+      <c r="A234" s="21"/>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="2"/>
+      <c r="A236" s="21"/>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="2"/>
+      <c r="A238" s="21"/>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="2"/>
+      <c r="A240" s="21"/>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="2"/>
+      <c r="A242" s="21"/>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="2"/>
+      <c r="A244" s="21"/>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="2"/>
+      <c r="A246" s="21"/>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="2"/>
+      <c r="A248" s="21"/>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="2"/>
+      <c r="A250" s="21"/>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="2"/>
+      <c r="A252" s="21"/>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="2"/>
+      <c r="A254" s="21"/>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="2"/>
+      <c r="A256" s="21"/>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="2"/>
+      <c r="A258" s="21"/>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="2"/>
+      <c r="A260" s="21"/>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="2"/>
+      <c r="A262" s="21"/>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264" s="2"/>
+      <c r="A264" s="21"/>
     </row>
     <row r="266" spans="1:1">
-      <c r="A266" s="2"/>
+      <c r="A266" s="21"/>
     </row>
     <row r="268" spans="1:1">
-      <c r="A268" s="2"/>
+      <c r="A268" s="21"/>
     </row>
     <row r="270" spans="1:1">
-      <c r="A270" s="2"/>
+      <c r="A270" s="21"/>
     </row>
     <row r="272" spans="1:1">
-      <c r="A272" s="2"/>
+      <c r="A272" s="21"/>
     </row>
     <row r="274" spans="1:1">
-      <c r="A274" s="2"/>
+      <c r="A274" s="21"/>
     </row>
     <row r="276" spans="1:1">
-      <c r="A276" s="2"/>
+      <c r="A276" s="21"/>
     </row>
     <row r="278" spans="1:1">
-      <c r="A278" s="2"/>
+      <c r="A278" s="21"/>
     </row>
     <row r="280" spans="1:1">
-      <c r="A280" s="2"/>
+      <c r="A280" s="21"/>
     </row>
     <row r="282" spans="1:1">
-      <c r="A282" s="2"/>
+      <c r="A282" s="21"/>
     </row>
     <row r="284" spans="1:1">
-      <c r="A284" s="2"/>
+      <c r="A284" s="21"/>
     </row>
     <row r="286" spans="1:1">
-      <c r="A286" s="2"/>
+      <c r="A286" s="21"/>
     </row>
     <row r="288" spans="1:1">
-      <c r="A288" s="2"/>
+      <c r="A288" s="21"/>
     </row>
     <row r="290" spans="1:1">
-      <c r="A290" s="2"/>
+      <c r="A290" s="21"/>
     </row>
     <row r="292" spans="1:1">
-      <c r="A292" s="2"/>
+      <c r="A292" s="21"/>
     </row>
     <row r="294" spans="1:1">
-      <c r="A294" s="2"/>
+      <c r="A294" s="21"/>
     </row>
     <row r="296" spans="1:1">
-      <c r="A296" s="2"/>
+      <c r="A296" s="21"/>
     </row>
     <row r="298" spans="1:1">
-      <c r="A298" s="2"/>
+      <c r="A298" s="21"/>
     </row>
     <row r="300" spans="1:1">
-      <c r="A300" s="2"/>
+      <c r="A300" s="21"/>
     </row>
     <row r="302" spans="1:1">
-      <c r="A302" s="2"/>
+      <c r="A302" s="21"/>
     </row>
     <row r="304" spans="1:1">
-      <c r="A304" s="2"/>
+      <c r="A304" s="21"/>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306" s="2"/>
+      <c r="A306" s="21"/>
     </row>
     <row r="308" spans="1:1">
-      <c r="A308" s="2"/>
+      <c r="A308" s="21"/>
     </row>
     <row r="310" spans="1:1">
-      <c r="A310" s="2"/>
+      <c r="A310" s="21"/>
     </row>
     <row r="312" spans="1:1">
-      <c r="A312" s="2"/>
+      <c r="A312" s="21"/>
     </row>
     <row r="314" spans="1:1">
-      <c r="A314" s="2"/>
+      <c r="A314" s="21"/>
     </row>
     <row r="316" spans="1:1">
-      <c r="A316" s="2"/>
+      <c r="A316" s="21"/>
     </row>
     <row r="318" spans="1:1">
-      <c r="A318" s="2"/>
+      <c r="A318" s="21"/>
     </row>
     <row r="320" spans="1:1">
-      <c r="A320" s="2"/>
+      <c r="A320" s="21"/>
     </row>
     <row r="322" spans="1:1">
-      <c r="A322" s="2"/>
+      <c r="A322" s="21"/>
     </row>
     <row r="324" spans="1:1">
-      <c r="A324" s="2"/>
+      <c r="A324" s="21"/>
     </row>
     <row r="326" spans="1:1">
-      <c r="A326" s="2"/>
+      <c r="A326" s="21"/>
     </row>
     <row r="328" spans="1:1">
-      <c r="A328" s="2"/>
+      <c r="A328" s="21"/>
     </row>
     <row r="330" spans="1:1">
-      <c r="A330" s="2"/>
+      <c r="A330" s="21"/>
     </row>
     <row r="332" spans="1:1">
-      <c r="A332" s="2"/>
+      <c r="A332" s="21"/>
     </row>
     <row r="334" spans="1:1">
-      <c r="A334" s="2"/>
+      <c r="A334" s="21"/>
     </row>
     <row r="336" spans="1:1">
-      <c r="A336" s="2"/>
+      <c r="A336" s="21"/>
     </row>
     <row r="338" spans="1:1">
-      <c r="A338" s="2"/>
+      <c r="A338" s="21"/>
     </row>
     <row r="340" spans="1:1">
-      <c r="A340" s="2"/>
+      <c r="A340" s="21"/>
     </row>
     <row r="342" spans="1:1">
-      <c r="A342" s="2"/>
+      <c r="A342" s="21"/>
     </row>
     <row r="344" spans="1:1">
-      <c r="A344" s="2"/>
+      <c r="A344" s="21"/>
     </row>
     <row r="346" spans="1:1">
-      <c r="A346" s="2"/>
+      <c r="A346" s="21"/>
     </row>
     <row r="348" spans="1:1">
-      <c r="A348" s="2"/>
+      <c r="A348" s="21"/>
     </row>
     <row r="350" spans="1:1">
-      <c r="A350" s="2"/>
+      <c r="A350" s="21"/>
     </row>
     <row r="352" spans="1:1">
-      <c r="A352" s="2"/>
+      <c r="A352" s="21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -3783,15 +4864,667 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="55" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" ht="15"/>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" ht="35.25" customHeight="1" spans="1:3">
+      <c r="A4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:3">
+      <c r="A5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" ht="23.25" customHeight="1" spans="1:3">
+      <c r="A9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" ht="24.75" customHeight="1" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" ht="15"/>
+    <row r="14" customHeight="1" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" ht="22.5" customHeight="1" spans="1:3">
+      <c r="A15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" ht="15" spans="1:3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" ht="15"/>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="12" t="e">
+        <f>幸运+支援效果</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" ht="15"/>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" customHeight="1" spans="1:3">
+      <c r="A34" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:3">
+      <c r="A36" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" customHeight="1" spans="1:3">
+      <c r="A38" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:3">
+      <c r="A42" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" customHeight="1" spans="1:3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" ht="15" spans="1:3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" ht="15"/>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="7">
+        <v>10</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="7">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>10</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="7">
+        <v>5</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="7">
+        <v>20</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="7">
+        <v>10</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="7">
+        <v>1</v>
+      </c>
+      <c r="C57" s="7">
+        <v>15</v>
+      </c>
+      <c r="D57" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="7">
+        <v>2</v>
+      </c>
+      <c r="C58" s="7">
+        <v>20</v>
+      </c>
+      <c r="D58" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="11">
+        <v>2</v>
+      </c>
+      <c r="C59" s="11">
+        <v>20</v>
+      </c>
+      <c r="D59" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" ht="15"/>
+    <row r="63" spans="1:4">
+      <c r="A63" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" ht="15"/>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" ht="15" spans="1:2">
+      <c r="A75" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C16:C18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>

</xml_diff>